<commit_message>
Actualizada matriz de elementos
</commit_message>
<xml_diff>
--- a/scripts/teselas/3ProcesoUnionDatos/lib/matriz_elementos.xlsx
+++ b/scripts/teselas/3ProcesoUnionDatos/lib/matriz_elementos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="100">
   <si>
     <t xml:space="preserve">elementos</t>
   </si>
@@ -65,6 +65,42 @@
   </si>
   <si>
     <t xml:space="preserve">construccion_pol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_carreteras_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_ferrocarril_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_hidrografia_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_lamina_agua_pol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_nombre_hidrografia_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_nombre_hidrografia_pol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_orografia_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_orografia_pol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_orografia_pto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_nombre_poblacion_pto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_territorios_lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contexto_territorios_pol</t>
   </si>
   <si>
     <t xml:space="preserve">edificio_pol</t>
@@ -404,15 +440,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.43"/>
@@ -580,41 +616,41 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>16</v>
@@ -625,130 +661,130 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -757,72 +793,72 @@
         <v>7</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="B19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="B20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>7</v>
@@ -831,18 +867,18 @@
         <v>7</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>7</v>
@@ -857,12 +893,12 @@
         <v>8</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>7</v>
@@ -877,12 +913,12 @@
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>7</v>
@@ -894,15 +930,15 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>7</v>
@@ -911,18 +947,18 @@
         <v>7</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>7</v>
@@ -931,18 +967,18 @@
         <v>7</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>7</v>
@@ -951,18 +987,18 @@
         <v>7</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>7</v>
@@ -971,18 +1007,18 @@
         <v>7</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>7</v>
@@ -991,18 +1027,18 @@
         <v>7</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>7</v>
@@ -1011,18 +1047,18 @@
         <v>7</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>7</v>
@@ -1031,18 +1067,18 @@
         <v>7</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>7</v>
@@ -1051,18 +1087,18 @@
         <v>7</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>7</v>
@@ -1071,18 +1107,18 @@
         <v>7</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>7</v>
@@ -1097,12 +1133,12 @@
         <v>8</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>7</v>
@@ -1111,18 +1147,18 @@
         <v>7</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>7</v>
@@ -1134,15 +1170,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>7</v>
@@ -1151,18 +1187,18 @@
         <v>7</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>7</v>
@@ -1171,18 +1207,18 @@
         <v>7</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>7</v>
@@ -1191,18 +1227,18 @@
         <v>7</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>7</v>
@@ -1217,12 +1253,12 @@
         <v>8</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>7</v>
@@ -1231,18 +1267,18 @@
         <v>7</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>7</v>
@@ -1257,12 +1293,12 @@
         <v>8</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>7</v>
@@ -1271,18 +1307,18 @@
         <v>7</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>7</v>
@@ -1291,18 +1327,18 @@
         <v>7</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>7</v>
@@ -1311,10 +1347,10 @@
         <v>7</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>56</v>
@@ -1357,12 +1393,12 @@
         <v>8</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>7</v>
@@ -1377,12 +1413,12 @@
         <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>7</v>
@@ -1397,12 +1433,12 @@
         <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>7</v>
@@ -1417,12 +1453,12 @@
         <v>8</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>7</v>
@@ -1437,12 +1473,12 @@
         <v>8</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>7</v>
@@ -1457,12 +1493,12 @@
         <v>8</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>7</v>
@@ -1471,18 +1507,18 @@
         <v>7</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>7</v>
@@ -1491,18 +1527,18 @@
         <v>7</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>7</v>
@@ -1511,18 +1547,18 @@
         <v>7</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>7</v>
@@ -1534,15 +1570,15 @@
         <v>7</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>7</v>
@@ -1554,15 +1590,15 @@
         <v>7</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>7</v>
@@ -1571,18 +1607,18 @@
         <v>7</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>7</v>
@@ -1597,12 +1633,12 @@
         <v>8</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>7</v>
@@ -1611,18 +1647,18 @@
         <v>7</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>7</v>
@@ -1651,7 +1687,7 @@
         <v>7</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>8</v>
@@ -1691,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>8</v>
@@ -1731,7 +1767,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>8</v>
@@ -1751,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>8</v>
@@ -1785,10 +1821,10 @@
         <v>83</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>7</v>
@@ -1831,7 +1867,7 @@
         <v>7</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>8</v>
@@ -1851,7 +1887,7 @@
         <v>7</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>8</v>
@@ -1871,15 +1907,256 @@
         <v>7</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>